<commit_message>
update 23 mar 22
added word2vec
</commit_message>
<xml_diff>
--- a/farmers_protest_ajay_5_march/analysis/search_analysis.xlsx
+++ b/farmers_protest_ajay_5_march/analysis/search_analysis.xlsx
@@ -10,7 +10,7 @@
     <sheet name="search_analysis" sheetId="1" r:id="rId1"/>
     <sheet name="ch_freq" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -12263,24 +12263,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="173650304"/>
-        <c:axId val="173652992"/>
+        <c:axId val="141585792"/>
+        <c:axId val="141829248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="173650304"/>
+        <c:axId val="141585792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173652992"/>
+        <c:crossAx val="141829248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173652992"/>
+        <c:axId val="141829248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12288,7 +12288,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173650304"/>
+        <c:crossAx val="141585792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12301,7 +12301,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -30974,7 +30974,7 @@
   <dimension ref="A1:B290"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>